<commit_message>
Updated with sjPlot code for outputting figures and table summaries of regression
</commit_message>
<xml_diff>
--- a/lm_models.xlsx
+++ b/lm_models.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t xml:space="preserve">
 </t>
@@ -126,7 +126,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">119 (118 to 121)</t>
+    <t xml:space="preserve">119 (118 to 119)</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -135,16 +135,16 @@
     <t xml:space="preserve">—</t>
   </si>
   <si>
-    <t xml:space="preserve">3.3 (1.8 to 4.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.8 (4.0 to 7.6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.4 (2.3 to 6.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.9 (6.2 to 12)</t>
+    <t xml:space="preserve">3.8 (2.7 to 4.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.1 (3.9 to 6.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.7 (3.3 to 6.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.9 (6.1 to 9.8)</t>
   </si>
   <si>
     <t xml:space="preserve">p-value
@@ -158,99 +158,102 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">110 (109 to 112)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.3 (0.92 to 3.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.0 (2.4 to 5.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.9 (1.0 to 4.8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.3 (0.80 to 5.8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.9 (2.1 to 5.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.0 (5.3 to 8.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 (11 to 15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 (14 to 19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 (21 to 26)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.3 (2.2 to 4.4)</t>
+    <t xml:space="preserve">109 (108 to 110)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2 (2.2 to 4.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9 (2.7 to 5.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.2 (1.9 to 4.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7 (1.9 to 5.4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0 (2.8 to 5.2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.7 (5.5 to 7.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13 (11 to 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 (14 to 17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24 (22 to 25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0 (3.2 to 4.8)</t>
   </si>
   <si>
     <t xml:space="preserve">Model 3
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2.1 (0.71 to 3.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.7 (2.1 to 5.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7 (0.79 to 4.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.8 (1.1 to 6.4)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.8 (5.1 to 8.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 (14 to 19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.2 (2.4 to 6.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.94 (-2.8 to 0.91)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.1 (-3.2 to 1.0)</t>
+    <t xml:space="preserve">2.9 (1.9 to 3.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.4 (2.3 to 4.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7 (1.3 to 4.0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6 (1.8 to 5.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1 (2.9 to 5.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1 (3.3 to 4.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4 (3.1 to 5.7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.03 (-1.2 to 1.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.3 (-2.8 to 0.24)</t>
   </si>
   <si>
     <t xml:space="preserve">Model 4
 </t>
   </si>
   <si>
-    <t xml:space="preserve">2.1 (0.68 to 3.5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.7 (0.76 to 4.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.9 (1.5 to 4.3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4.3 (1.7 to 6.9)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7.0 (4.4 to 9.7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.5 (-4.0 to 1.1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5 (-0.02 to 5.0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.9 (-5.8 to 0.07)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3.7 (0.69 to 6.6)</t>
+    <t xml:space="preserve">3.7 (1.9 to 5.5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.1 (2.8 to 5.3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.6 (5.4 to 7.8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.7 (2.8 to 4.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.8 (3.0 to 6.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.7 (5.9 to 9.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.72 (-2.5 to 1.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4 (2.7 to 6.1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.0 (-5.1 to -0.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.3 (2.1 to 6.5)</t>
   </si>
 </sst>
 </file>
@@ -865,20 +868,20 @@
       <c r="D6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="10" t="n">
-        <v>0.001</v>
+      <c r="E6" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="10" t="n">
-        <v>0.003</v>
+      <c r="G6" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="10" t="n">
-        <v>0.004</v>
+        <v>58</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" ht="NA" customHeight="1">
@@ -923,20 +926,20 @@
       <c r="D8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="10" t="n">
-        <v>0.003</v>
+      <c r="E8" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="10" t="n">
-        <v>0.006</v>
+      <c r="G8" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="10" t="n">
-        <v>0.006</v>
+        <v>60</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="9" ht="NA" customHeight="1">
@@ -952,20 +955,20 @@
       <c r="D9" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="10" t="n">
-        <v>0.01</v>
+      <c r="E9" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="10" t="n">
-        <v>0.006</v>
+      <c r="G9" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>0.005</v>
+        <v>68</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" ht="NA" customHeight="1">
@@ -1043,13 +1046,13 @@
         <v>44</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>44</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>44</v>
@@ -1072,13 +1075,13 @@
         <v>44</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G13" s="10" t="s">
         <v>44</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>44</v>
@@ -1130,13 +1133,13 @@
         <v>44</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>44</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>44</v>
@@ -1246,7 +1249,7 @@
         <v>44</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>44</v>
@@ -1365,7 +1368,7 @@
         <v>65</v>
       </c>
       <c r="G23" s="10" t="n">
-        <v>0.32</v>
+        <v>0.96</v>
       </c>
       <c r="H23" s="10" t="s">
         <v>37</v>
@@ -1394,7 +1397,7 @@
         <v>66</v>
       </c>
       <c r="G24" s="10" t="n">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>37</v>
@@ -1484,7 +1487,7 @@
         <v>37</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>44</v>
@@ -1513,10 +1516,10 @@
         <v>37</v>
       </c>
       <c r="H28" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I28" s="10" t="n">
-        <v>0.001</v>
+        <v>72</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" ht="NA" customHeight="1">
@@ -1542,7 +1545,7 @@
         <v>37</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>44</v>
@@ -1571,10 +1574,10 @@
         <v>37</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I30" s="10" t="n">
-        <v>0.26</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="31" ht="NA" customHeight="1">
@@ -1600,10 +1603,10 @@
         <v>37</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="I31" s="10" t="n">
-        <v>0.052</v>
+        <v>75</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="32" ht="NA" customHeight="1">
@@ -1629,10 +1632,10 @@
         <v>37</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I32" s="10" t="n">
-        <v>0.055</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="33" ht="NA" customHeight="1">
@@ -1658,10 +1661,10 @@
         <v>37</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I33" s="11" t="n">
-        <v>0.016</v>
+        <v>77</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" ht="NA" customHeight="1">

</xml_diff>